<commit_message>
add encoders and ultrasounds pins
</commit_message>
<xml_diff>
--- a/docs/pinout.xlsx
+++ b/docs/pinout.xlsx
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t xml:space="preserve">Robot</t>
   </si>
   <si>
     <t xml:space="preserve">BCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3V array</t>
   </si>
   <si>
     <r>
@@ -36,6 +39,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3V
 </t>
@@ -46,6 +50,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Power</t>
     </r>
@@ -58,6 +63,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5V
 </t>
@@ -68,15 +74,16 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Power</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ultrasounds power (using array)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Encoder 1 </t>
+    <t xml:space="preserve">5V array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder 1 White </t>
   </si>
   <si>
     <r>
@@ -86,6 +93,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">GPIO2
 </t>
@@ -96,12 +104,13 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SDA1 I2C</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">encoders power (using array)</t>
+    <t xml:space="preserve">Encoder 1 Yellow</t>
   </si>
   <si>
     <r>
@@ -111,6 +120,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">GPIO3
 </t>
@@ -121,24 +131,51 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SCL1 I2C</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultrasounds ground (using array)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO4
+</t>
   </si>
   <si>
     <r>
       <rPr>
         <b val="true"/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ground
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ultrasounds ground (using array)</t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO14
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UART0_TXD</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder 2 White </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground array</t>
   </si>
   <si>
     <r>
@@ -148,10 +185,31 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO4
-</t>
-    </r>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO15
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">UART0_RXD</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder 2 Yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound Front trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO17
+</t>
   </si>
   <si>
     <r>
@@ -161,8 +219,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO14
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO18
 </t>
     </r>
     <r>
@@ -171,12 +230,63 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">UART0_TXD</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">encoders ground (using array)</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PCM_CLK</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound Front echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO27
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 1 ENABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO22
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO23
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 2 ENABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO24
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 1 DIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound FL trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound FL echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO9
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO25
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 2 DIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO11
+</t>
   </si>
   <si>
     <r>
@@ -186,8 +296,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO15
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO8
 </t>
     </r>
     <r>
@@ -196,9 +307,13 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">UART0_RXD</t>
-    </r>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SPI0_CE0_N</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound FR trigger</t>
   </si>
   <si>
     <r>
@@ -208,10 +323,27 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO17
-</t>
-    </r>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO7
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SPI0_CE1_N</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound FR echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORBIDDEN</t>
   </si>
   <si>
     <r>
@@ -221,8 +353,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO18
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO0 (ID_SD)
 </t>
     </r>
     <r>
@@ -231,8 +364,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">PCM_CLK</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I2C ID EEPROM</t>
     </r>
   </si>
   <si>
@@ -243,13 +377,35 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO27
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 1 ENABLE</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO1 (ID_SC)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I2C ID EEPROM</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 1 FAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO5
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 2 FAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO6
+</t>
   </si>
   <si>
     <r>
@@ -259,10 +415,27 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO22
-</t>
-    </r>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO12
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pwm0</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 1 PWM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor 2 PWM</t>
   </si>
   <si>
     <r>
@@ -272,322 +445,53 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO23
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 2 ENABLE</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GPIO13
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO24
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 1 DIR</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO10
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO9
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO25
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 2 DIR</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO11
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO8
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">SPI0_CE0_N</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO7
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">SPI0_CE1_N</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">FORBIDDEN</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO0 (ID_SD)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">I2C ID EEPROM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO1 (ID_SC)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">I2C ID EEPROM</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 1 FAULT</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO5
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 2 FAULT</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO6
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO12
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Pwm0</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 1 PWM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motor 2 PWM</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO13
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pwm1</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO19
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO16
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO26
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO20
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">GPIO21
-</t>
-    </r>
+    <t xml:space="preserve">Ultrasound RL trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO19
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO16
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound RR trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound RL echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO26
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO20
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasound RR echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIO21
+</t>
   </si>
   <si>
     <t xml:space="preserve">Pins</t>
@@ -644,6 +548,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -666,6 +571,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -674,6 +580,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -681,12 +588,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -694,6 +603,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -701,11 +611,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -714,29 +631,28 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -744,6 +660,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -890,7 +807,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -995,23 +912,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1035,7 +956,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1091,7 +1012,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1103,7 +1024,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1191,10 +1112,10 @@
   <dimension ref="C1:O44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.37"/>
@@ -1254,8 +1175,11 @@
       <c r="M3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="D4" s="13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="15"/>
@@ -1271,10 +1195,10 @@
       <c r="L4" s="8"/>
       <c r="M4" s="4"/>
       <c r="N4" s="20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,10 +1216,10 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="23"/>
@@ -1311,10 +1235,7 @@
       <c r="L6" s="8"/>
       <c r="M6" s="4"/>
       <c r="N6" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,8 +1252,11 @@
       <c r="N7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="26" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="23"/>
@@ -1341,17 +1265,17 @@
         <v>5</v>
       </c>
       <c r="I8" s="18"/>
-      <c r="J8" s="26" t="n">
+      <c r="J8" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="30" t="s">
-        <v>9</v>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,30 +1291,33 @@
       <c r="M9" s="4"/>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="31" t="s">
-        <v>11</v>
+    <row r="10" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="32" t="s">
+        <v>12</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
-      <c r="H10" s="32" t="n">
+      <c r="H10" s="33" t="n">
         <v>7</v>
       </c>
       <c r="I10" s="18"/>
-      <c r="J10" s="33" t="n">
+      <c r="J10" s="34" t="n">
         <v>8</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="8"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="34" t="s">
-        <v>12</v>
+      <c r="N10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="15"/>
       <c r="G11" s="16"/>
       <c r="H11" s="18"/>
@@ -1403,26 +1330,29 @@
     </row>
     <row r="12" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="37"/>
+        <v>15</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="38"/>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
-      <c r="H12" s="26" t="n">
+      <c r="H12" s="27" t="n">
         <v>9</v>
       </c>
       <c r="I12" s="18"/>
-      <c r="J12" s="33" t="n">
+      <c r="J12" s="34" t="n">
         <v>10</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="8"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="34" t="s">
-        <v>14</v>
+      <c r="N12" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="26" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,33 +1360,36 @@
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="38"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="18"/>
-      <c r="J13" s="38"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="11"/>
       <c r="L13" s="8"/>
       <c r="M13" s="4"/>
       <c r="N13" s="21"/>
     </row>
-    <row r="14" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="31" t="s">
-        <v>15</v>
+    <row r="14" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>19</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
-      <c r="H14" s="32" t="n">
+      <c r="H14" s="33" t="n">
         <v>11</v>
       </c>
       <c r="I14" s="18"/>
-      <c r="J14" s="32" t="n">
+      <c r="J14" s="33" t="n">
         <v>12</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="8"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="39" t="s">
-        <v>16</v>
+      <c r="N14" s="40" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,25 +1405,28 @@
       <c r="M15" s="4"/>
       <c r="N15" s="21"/>
     </row>
-    <row r="16" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="31" t="s">
-        <v>17</v>
+    <row r="16" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>22</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
-      <c r="H16" s="32" t="n">
+      <c r="H16" s="33" t="n">
         <v>13</v>
       </c>
       <c r="I16" s="18"/>
-      <c r="J16" s="26" t="n">
+      <c r="J16" s="27" t="n">
         <v>14</v>
       </c>
-      <c r="K16" s="27"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="30" t="s">
-        <v>9</v>
+      <c r="K16" s="28"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,29 +1444,29 @@
     </row>
     <row r="18" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>24</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="32" t="n">
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="33" t="n">
         <v>15</v>
       </c>
       <c r="I18" s="18"/>
-      <c r="J18" s="32" t="n">
+      <c r="J18" s="33" t="n">
         <v>16</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="8"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="39" t="s">
-        <v>20</v>
+      <c r="N18" s="40" t="s">
+        <v>25</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1484,7 @@
     </row>
     <row r="20" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
@@ -1557,17 +1493,17 @@
         <v>17</v>
       </c>
       <c r="I20" s="18"/>
-      <c r="J20" s="32" t="n">
+      <c r="J20" s="33" t="n">
         <v>18</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="8"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="39" t="s">
-        <v>22</v>
+      <c r="N20" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,25 +1519,28 @@
       <c r="M21" s="4"/>
       <c r="N21" s="21"/>
     </row>
-    <row r="22" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="42" t="s">
-        <v>24</v>
+    <row r="22" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>30</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="23"/>
       <c r="G22" s="24"/>
-      <c r="H22" s="33" t="n">
+      <c r="H22" s="34" t="n">
         <v>19</v>
       </c>
       <c r="I22" s="18"/>
-      <c r="J22" s="26" t="n">
+      <c r="J22" s="27" t="n">
         <v>20</v>
       </c>
-      <c r="K22" s="27"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="30" t="s">
-        <v>9</v>
+      <c r="K22" s="28"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,28 +1556,31 @@
       <c r="M23" s="4"/>
       <c r="N23" s="21"/>
     </row>
-    <row r="24" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="42" t="s">
-        <v>25</v>
+    <row r="24" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="23"/>
       <c r="G24" s="24"/>
-      <c r="H24" s="33" t="n">
+      <c r="H24" s="34" t="n">
         <v>21</v>
       </c>
       <c r="I24" s="18"/>
-      <c r="J24" s="43" t="n">
+      <c r="J24" s="44" t="n">
         <v>22</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="8"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="44" t="s">
-        <v>26</v>
+      <c r="N24" s="45" t="s">
+        <v>33</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,25 +1596,28 @@
       <c r="M25" s="4"/>
       <c r="N25" s="21"/>
     </row>
-    <row r="26" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="42" t="s">
-        <v>28</v>
+    <row r="26" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="43" t="s">
+        <v>35</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="23"/>
       <c r="G26" s="24"/>
-      <c r="H26" s="33" t="n">
+      <c r="H26" s="34" t="n">
         <v>23</v>
       </c>
       <c r="I26" s="18"/>
-      <c r="J26" s="33" t="n">
+      <c r="J26" s="34" t="n">
         <v>24</v>
       </c>
       <c r="K26" s="11"/>
       <c r="L26" s="8"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="34" t="s">
-        <v>29</v>
+      <c r="N26" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,24 +1634,27 @@
       <c r="N27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="26" t="n">
+      <c r="D28" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="38"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="27" t="n">
         <v>25</v>
       </c>
       <c r="I28" s="18"/>
-      <c r="J28" s="33" t="n">
+      <c r="J28" s="34" t="n">
         <v>26</v>
       </c>
       <c r="K28" s="11"/>
       <c r="L28" s="8"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="34" t="s">
-        <v>30</v>
+      <c r="N28" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="O28" s="26" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,29 +1672,29 @@
     </row>
     <row r="30" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>41</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="23"/>
       <c r="G30" s="24"/>
-      <c r="H30" s="48" t="n">
+      <c r="H30" s="49" t="n">
         <v>27</v>
       </c>
       <c r="I30" s="18"/>
-      <c r="J30" s="48" t="n">
+      <c r="J30" s="49" t="n">
         <v>28</v>
       </c>
       <c r="K30" s="11"/>
       <c r="L30" s="8"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="49" t="s">
-        <v>33</v>
+      <c r="N30" s="50" t="s">
+        <v>42</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,26 +1712,26 @@
     </row>
     <row r="32" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="23"/>
       <c r="G32" s="24"/>
-      <c r="H32" s="32" t="n">
+      <c r="H32" s="33" t="n">
         <v>29</v>
       </c>
       <c r="I32" s="18"/>
-      <c r="J32" s="26" t="n">
+      <c r="J32" s="27" t="n">
         <v>30</v>
       </c>
-      <c r="K32" s="27"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="30" t="s">
-        <v>9</v>
+      <c r="K32" s="28"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,29 +1749,29 @@
     </row>
     <row r="34" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>46</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="23"/>
       <c r="G34" s="24"/>
-      <c r="H34" s="32" t="n">
+      <c r="H34" s="33" t="n">
         <v>31</v>
       </c>
       <c r="I34" s="18"/>
-      <c r="J34" s="32" t="n">
+      <c r="J34" s="33" t="n">
         <v>32</v>
       </c>
       <c r="K34" s="11"/>
       <c r="L34" s="8"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="39" t="s">
-        <v>38</v>
+      <c r="N34" s="40" t="s">
+        <v>47</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,9 +1779,9 @@
       <c r="E35" s="14"/>
       <c r="F35" s="15"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="38"/>
+      <c r="H35" s="39"/>
       <c r="I35" s="18"/>
-      <c r="J35" s="38"/>
+      <c r="J35" s="39"/>
       <c r="K35" s="11"/>
       <c r="L35" s="8"/>
       <c r="M35" s="4"/>
@@ -1841,26 +1789,26 @@
     </row>
     <row r="36" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>41</v>
+        <v>49</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="23"/>
       <c r="G36" s="24"/>
-      <c r="H36" s="32" t="n">
+      <c r="H36" s="33" t="n">
         <v>33</v>
       </c>
       <c r="I36" s="18"/>
-      <c r="J36" s="26" t="n">
+      <c r="J36" s="27" t="n">
         <v>34</v>
       </c>
-      <c r="K36" s="27"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="30" t="s">
-        <v>9</v>
+      <c r="K36" s="28"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,25 +1824,31 @@
       <c r="M37" s="4"/>
       <c r="N37" s="21"/>
     </row>
-    <row r="38" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="31" t="s">
-        <v>42</v>
+    <row r="38" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>52</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="23"/>
       <c r="G38" s="24"/>
-      <c r="H38" s="32" t="n">
+      <c r="H38" s="33" t="n">
         <v>35</v>
       </c>
       <c r="I38" s="18"/>
-      <c r="J38" s="32" t="n">
+      <c r="J38" s="33" t="n">
         <v>36</v>
       </c>
       <c r="K38" s="11"/>
       <c r="L38" s="8"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="39" t="s">
-        <v>43</v>
+      <c r="N38" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="O38" s="26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,25 +1864,31 @@
       <c r="M39" s="4"/>
       <c r="N39" s="21"/>
     </row>
-    <row r="40" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="31" t="s">
-        <v>44</v>
+    <row r="40" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>56</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="23"/>
       <c r="G40" s="24"/>
-      <c r="H40" s="32" t="n">
+      <c r="H40" s="33" t="n">
         <v>37</v>
       </c>
       <c r="I40" s="18"/>
-      <c r="J40" s="32" t="n">
+      <c r="J40" s="33" t="n">
         <v>38</v>
       </c>
       <c r="K40" s="11"/>
       <c r="L40" s="8"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="39" t="s">
-        <v>45</v>
+      <c r="N40" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="O40" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="20.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,51 +1905,51 @@
       <c r="N41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="26" t="n">
+      <c r="D42" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="38"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="27" t="n">
         <v>39</v>
       </c>
       <c r="I42" s="18"/>
-      <c r="J42" s="32" t="n">
+      <c r="J42" s="33" t="n">
         <v>40</v>
       </c>
       <c r="K42" s="11"/>
       <c r="L42" s="8"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="39" t="s">
-        <v>46</v>
+      <c r="N42" s="40" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="51"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="52"/>
       <c r="K43" s="11"/>
       <c r="L43" s="8"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="52"/>
+      <c r="N43" s="53"/>
     </row>
     <row r="44" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="54"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="55"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="52"/>
+      <c r="N44" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2016,7 +1976,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.08"/>
@@ -2024,18 +1984,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>40</v>
@@ -2043,7 +2003,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -2051,7 +2011,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -2059,7 +2019,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>8</v>
@@ -2067,7 +2027,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
@@ -2075,7 +2035,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B2-SUM(B3:B6)</f>
@@ -2084,13 +2044,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2</v>
@@ -2102,13 +2062,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
@@ -2120,13 +2080,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>5</v>

</xml_diff>